<commit_message>
SubstanceInFuelMix now running with the CO2 Market again
</commit_message>
<xml_diff>
--- a/resources/configurations/EMLAB config.xlsx
+++ b/resources/configurations/EMLAB config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\workspace\Spine_EMLab_COMPETES\resources\configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E0CB91-39BC-4BCC-A3BB-886194FE67A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682DFD64-66A1-4EF0-9F74-8765E1D7C5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import Priorities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>object_class_name</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>EnergyProducers</t>
+  </si>
+  <si>
+    <t>PowerGeneratingTechnologyFuel</t>
   </si>
 </sst>
 </file>
@@ -375,15 +378,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -466,6 +469,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>